<commit_message>
working on adding upper limits to target table.
</commit_message>
<xml_diff>
--- a/nutrition_database_for_app.xlsx
+++ b/nutrition_database_for_app.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-6440" yWindow="-17220" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="8320" yWindow="-21420" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>UL Zinc(mg/d)</t>
   </si>
   <si>
-    <t>UL Flouride(µg/d)</t>
-  </si>
-  <si>
     <t>Vit K (μg/d)(430)</t>
   </si>
   <si>
@@ -179,10 +176,13 @@
     <t>Vit C (mg/d)(401)</t>
   </si>
   <si>
-    <t>Flouride (µg/d)(313)</t>
-  </si>
-  <si>
     <t>Biotin (μg/d)</t>
+  </si>
+  <si>
+    <t>Fluoride (µg/d)(313)</t>
+  </si>
+  <si>
+    <t>UL Fluoride(µg/d)</t>
   </si>
 </sst>
 </file>
@@ -237,8 +237,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="447">
+  <cellStyleXfs count="477">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -690,7 +720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="447">
+  <cellStyles count="477">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -914,6 +944,21 @@
     <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1137,6 +1182,21 @@
     <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1468,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I23"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1488,139 +1548,139 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>45</v>
-      </c>
-      <c r="L1" t="s">
-        <v>46</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
-        <v>36</v>
-      </c>
       <c r="Q1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R1" t="s">
         <v>11</v>
       </c>
       <c r="S1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T1" t="s">
         <v>12</v>
       </c>
       <c r="U1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AB1" t="s">
         <v>52</v>
       </c>
       <c r="AC1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="AD1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AE1" t="s">
         <v>13</v>
       </c>
       <c r="AF1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AG1" t="s">
         <v>14</v>
       </c>
       <c r="AH1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AI1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AJ1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AK1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AL1" t="s">
         <v>15</v>
       </c>
       <c r="AM1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AN1" t="s">
         <v>16</v>
       </c>
       <c r="AO1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP1" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" t="s">
-        <v>26</v>
-      </c>
       <c r="AQ1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AR1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS1" t="s">
         <v>19</v>
       </c>
-      <c r="AS1" t="s">
-        <v>20</v>
-      </c>
       <c r="AT1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU1" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" t="s">
-        <v>43</v>
-      </c>
       <c r="AV1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:48">

</xml_diff>